<commit_message>
Corrected the .csv file (empty duplicated rows, values on 04/09 wrongly copied on the 20/08). Produced a draft but apparently correct set of plots with the cumulated values of collected N. Still missing the line(s) with the application values but that should be easy peasy lemon squeezy.
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_fieldlab/old/15N_Ndep_db.xlsx
+++ b/15N_experiment/15N_fieldlab/old/15N_Ndep_db.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1373890\Daniele_Repo\15N_experiment\15N_fieldlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1373890\Daniele_Repo\15N_experiment\15N_fieldlab\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -703,8 +703,8 @@
   <dimension ref="A1:Y119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,7 +1811,9 @@
       <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6">
+        <v>7</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1852,7 +1854,9 @@
       <c r="D27" s="6">
         <v>3</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6">
+        <v>6.25</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1895,7 +1899,9 @@
       <c r="D28" s="6">
         <v>3</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>6.75</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1937,6 +1943,9 @@
       <c r="D29" s="7">
         <v>3</v>
       </c>
+      <c r="E29" s="7">
+        <v>4.75</v>
+      </c>
       <c r="L29" s="30">
         <v>0.23899999999999999</v>
       </c>
@@ -1972,6 +1981,9 @@
       <c r="D30" s="7">
         <v>3</v>
       </c>
+      <c r="E30" s="7">
+        <v>4.7</v>
+      </c>
       <c r="L30" s="30">
         <v>0.19800000000000001</v>
       </c>
@@ -2004,6 +2016,9 @@
       </c>
       <c r="D31" s="7">
         <v>3</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2</v>
       </c>
       <c r="L31" s="30">
         <v>1.129</v>
@@ -2213,7 +2228,7 @@
         <v>7.5</v>
       </c>
       <c r="K37" s="6">
-        <v>7</v>
+        <v>31.5</v>
       </c>
       <c r="L37" s="30">
         <v>0.28899999999999998</v>
@@ -2237,6 +2252,22 @@
         <v>0.8</v>
       </c>
       <c r="S37" s="6"/>
+      <c r="U37" s="32">
+        <f>(H37-0.6078)/1.3756</f>
+        <v>6.1007560337307369</v>
+      </c>
+      <c r="V37" s="32">
+        <f t="shared" ref="V37" si="0">(I37-0.6078)/1.3756</f>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="W37" s="32">
+        <f t="shared" ref="W37" si="1">(J37-0.6078)/1.3756</f>
+        <v>5.0103227682465832</v>
+      </c>
+      <c r="X37" s="32">
+        <f t="shared" ref="X37:X42" si="2">(K37-0.6078)/1.3756</f>
+        <v>22.45725501599302</v>
+      </c>
     </row>
     <row r="38" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -2280,6 +2311,10 @@
         <v>1</v>
       </c>
       <c r="S38" s="6"/>
+      <c r="X38" s="32">
+        <f t="shared" si="2"/>
+        <v>17.005088688572261</v>
+      </c>
     </row>
     <row r="39" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -2323,6 +2358,10 @@
         <v>0.45</v>
       </c>
       <c r="S39" s="6"/>
+      <c r="X39" s="32">
+        <f t="shared" si="2"/>
+        <v>21.003343995347485</v>
+      </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -2359,6 +2398,10 @@
         <v>1</v>
       </c>
       <c r="S40" s="7"/>
+      <c r="X40" s="32">
+        <f t="shared" si="2"/>
+        <v>15.551177667926723</v>
+      </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -2395,6 +2438,10 @@
         <v>0.4</v>
       </c>
       <c r="S41" s="7"/>
+      <c r="X41" s="32">
+        <f t="shared" si="2"/>
+        <v>17.005088688572261</v>
+      </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -2432,6 +2479,10 @@
       </c>
       <c r="S42" s="7" t="s">
         <v>50</v>
+      </c>
+      <c r="X42" s="32">
+        <f t="shared" si="2"/>
+        <v>3.1929339924396629</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
@@ -2639,15 +2690,15 @@
         <v>26.092032567606864</v>
       </c>
       <c r="V48" s="32">
-        <f t="shared" ref="V48:V50" si="0">(I48-0.6078)/1.3756</f>
+        <f t="shared" ref="V48:V50" si="3">(I48-0.6078)/1.3756</f>
         <v>22.093777260831637</v>
       </c>
       <c r="W48" s="32">
-        <f t="shared" ref="W48:W49" si="1">(J48-0.6078)/1.3756</f>
+        <f t="shared" ref="W48:W49" si="4">(J48-0.6078)/1.3756</f>
         <v>17.005088688572261</v>
       </c>
       <c r="X48" s="32">
-        <f t="shared" ref="X48:X50" si="2">(K48-0.6078)/1.3756</f>
+        <f t="shared" ref="X48:X50" si="5">(K48-0.6078)/1.3756</f>
         <v>17.732044198895029</v>
       </c>
     </row>
@@ -2663,7 +2714,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="33">
-        <f t="shared" ref="E49:E50" si="3">SUM(U49:X49)</f>
+        <f t="shared" ref="E49:E50" si="6">SUM(U49:X49)</f>
         <v>74.562954347193966</v>
       </c>
       <c r="F49" s="6"/>
@@ -2699,15 +2750,15 @@
         <v>14.097266647281186</v>
       </c>
       <c r="V49" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>30.090287874382092</v>
       </c>
       <c r="W49" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13.370311136958419</v>
       </c>
       <c r="X49" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>17.005088688572261</v>
       </c>
     </row>
@@ -2723,7 +2774,7 @@
         <v>5</v>
       </c>
       <c r="E50" s="33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>82.559464960744407</v>
       </c>
       <c r="F50" s="6"/>
@@ -2755,11 +2806,11 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="U50" s="32">
-        <f t="shared" ref="U50" si="4">(H50-0.6078)/1.3756</f>
+        <f t="shared" ref="U50" si="7">(H50-0.6078)/1.3756</f>
         <v>18.458999709217796</v>
       </c>
       <c r="V50" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25.728554812445481</v>
       </c>
       <c r="W50" s="32">
@@ -2767,7 +2818,7 @@
         <v>25.728554812445481</v>
       </c>
       <c r="X50" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>12.64335562663565</v>
       </c>
     </row>
@@ -2817,7 +2868,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="33">
-        <f t="shared" ref="E52:E53" si="5">(H52-0.6078)/1.3756</f>
+        <f t="shared" ref="E52:E53" si="8">(H52-0.6078)/1.3756</f>
         <v>28.636376853736554</v>
       </c>
       <c r="H52" s="3">
@@ -2852,7 +2903,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>17.005088688572261</v>
       </c>
       <c r="H53" s="3">
@@ -3028,15 +3079,15 @@
         <v>11.916400116312882</v>
       </c>
       <c r="V59" s="32">
-        <f t="shared" ref="V59:V61" si="6">(I59-0.6078)/1.3756</f>
+        <f t="shared" ref="V59:V61" si="9">(I59-0.6078)/1.3756</f>
         <v>10.462489095667346</v>
       </c>
       <c r="W59" s="32">
-        <f t="shared" ref="W59:W60" si="7">(J59-0.6078)/1.3756</f>
+        <f t="shared" ref="W59:W60" si="10">(J59-0.6078)/1.3756</f>
         <v>11.189444605990115</v>
       </c>
       <c r="X59" s="32">
-        <f t="shared" ref="X59:X61" si="8">(K59-0.6078)/1.3756</f>
+        <f t="shared" ref="X59:X61" si="11">(K59-0.6078)/1.3756</f>
         <v>12.64335562663565</v>
       </c>
     </row>
@@ -3052,7 +3103,7 @@
         <v>6</v>
       </c>
       <c r="E60" s="33">
-        <f t="shared" ref="E60:E61" si="9">SUM(U60:X60)</f>
+        <f t="shared" ref="E60:E61" si="12">SUM(U60:X60)</f>
         <v>32.3995347484734</v>
       </c>
       <c r="F60" s="6"/>
@@ -3086,15 +3137,15 @@
         <v>6.1007560337307369</v>
       </c>
       <c r="V60" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>14.097266647281186</v>
       </c>
       <c r="W60" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.3738005234079678</v>
       </c>
       <c r="X60" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.8277115440535052</v>
       </c>
     </row>
@@ -3110,7 +3161,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>37.488223320732779</v>
       </c>
       <c r="F61" s="6"/>
@@ -3140,11 +3191,11 @@
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
       <c r="U61" s="32">
-        <f t="shared" ref="U61" si="10">(H61-0.6078)/1.3756</f>
+        <f t="shared" ref="U61" si="13">(H61-0.6078)/1.3756</f>
         <v>9.7355335853445784</v>
       </c>
       <c r="V61" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.7355335853445784</v>
       </c>
       <c r="W61" s="32">
@@ -3152,7 +3203,7 @@
         <v>11.916400116312882</v>
       </c>
       <c r="X61" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.1007560337307369</v>
       </c>
     </row>
@@ -3410,15 +3461,15 @@
         <v>12.64335562663565</v>
       </c>
       <c r="V70" s="32">
-        <f t="shared" ref="V70:V72" si="11">(I70-0.6078)/1.3756</f>
+        <f t="shared" ref="V70:V72" si="14">(I70-0.6078)/1.3756</f>
         <v>9.7355335853445784</v>
       </c>
       <c r="W70" s="32">
-        <f t="shared" ref="W70:W71" si="12">(J70-0.6078)/1.3756</f>
+        <f t="shared" ref="W70:W71" si="15">(J70-0.6078)/1.3756</f>
         <v>9.0085780750218092</v>
       </c>
       <c r="X70" s="32">
-        <f t="shared" ref="X70:X72" si="13">(K70-0.6078)/1.3756</f>
+        <f t="shared" ref="X70:X72" si="16">(K70-0.6078)/1.3756</f>
         <v>9.7355335853445784</v>
       </c>
     </row>
@@ -3434,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="E71" s="33">
-        <f t="shared" ref="E71:E72" si="14">SUM(U71:X71)</f>
+        <f t="shared" ref="E71:E72" si="17">SUM(U71:X71)</f>
         <v>41.123000872346616</v>
       </c>
       <c r="F71" s="6"/>
@@ -3468,15 +3519,15 @@
         <v>9.7355335853445784</v>
       </c>
       <c r="V71" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>9.0085780750218092</v>
       </c>
       <c r="W71" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>14.824222157603955</v>
       </c>
       <c r="X71" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>7.5546670543762735</v>
       </c>
     </row>
@@ -3492,7 +3543,7 @@
         <v>7</v>
       </c>
       <c r="E72" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>46.211689444605994</v>
       </c>
       <c r="F72" s="6"/>
@@ -3522,11 +3573,11 @@
       <c r="R72" s="6"/>
       <c r="S72" s="6"/>
       <c r="U72" s="32">
-        <f t="shared" ref="U72" si="15">(H72-0.6078)/1.3756</f>
+        <f t="shared" ref="U72" si="18">(H72-0.6078)/1.3756</f>
         <v>9.7355335853445784</v>
       </c>
       <c r="V72" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>12.64335562663565</v>
       </c>
       <c r="W72" s="32">
@@ -3534,7 +3585,7 @@
         <v>10.462489095667346</v>
       </c>
       <c r="X72" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>13.370311136958419</v>
       </c>
     </row>
@@ -3549,7 +3600,7 @@
         <v>7</v>
       </c>
       <c r="E73" s="33">
-        <f t="shared" ref="E73:E75" si="16">(H73-0.6078)/1.3756</f>
+        <f t="shared" ref="E73:E75" si="19">(H73-0.6078)/1.3756</f>
         <v>27.182465833091019</v>
       </c>
       <c r="H73" s="3">
@@ -3579,7 +3630,7 @@
         <v>7</v>
       </c>
       <c r="E74" s="33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>16.27813317824949</v>
       </c>
       <c r="H74" s="3">
@@ -3609,7 +3660,7 @@
         <v>7</v>
       </c>
       <c r="E75" s="33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>9.7355335853445784</v>
       </c>
       <c r="H75" s="3">
@@ -4397,15 +4448,15 @@
         <v>7.5546670543762735</v>
       </c>
       <c r="V103" s="32">
-        <f t="shared" ref="V103:X103" si="17">(I103-0.6078)/1.3756</f>
+        <f t="shared" ref="V103:X103" si="20">(I103-0.6078)/1.3756</f>
         <v>6.1007560337307369</v>
       </c>
       <c r="W103" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.3738005234079678</v>
       </c>
       <c r="X103" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.3738005234079678</v>
       </c>
     </row>
@@ -4421,7 +4472,7 @@
         <v>10</v>
       </c>
       <c r="E104" s="33">
-        <f t="shared" ref="E104:E105" si="18">SUM(U104:X104)</f>
+        <f t="shared" ref="E104:E105" si="21">SUM(U104:X104)</f>
         <v>22.222157603954638</v>
       </c>
       <c r="F104" s="6"/>
@@ -4457,15 +4508,15 @@
         <v>5.3738005234079678</v>
       </c>
       <c r="V104" s="32">
-        <f t="shared" ref="V104:V105" si="19">(I104-0.6078)/1.3756</f>
+        <f t="shared" ref="V104:V105" si="22">(I104-0.6078)/1.3756</f>
         <v>3.9198895027624312</v>
       </c>
       <c r="W104" s="32">
-        <f t="shared" ref="W104" si="20">(J104-0.6078)/1.3756</f>
+        <f t="shared" ref="W104" si="23">(J104-0.6078)/1.3756</f>
         <v>9.0085780750218092</v>
       </c>
       <c r="X104" s="32">
-        <f t="shared" ref="X104:X105" si="21">(K104-0.6078)/1.3756</f>
+        <f t="shared" ref="X104:X105" si="24">(K104-0.6078)/1.3756</f>
         <v>3.9198895027624312</v>
       </c>
     </row>
@@ -4481,7 +4532,7 @@
         <v>10</v>
       </c>
       <c r="E105" s="33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>25.129979645245715</v>
       </c>
       <c r="F105" s="6"/>
@@ -4513,11 +4564,11 @@
         <v>4</v>
       </c>
       <c r="U105" s="32">
-        <f t="shared" ref="U105" si="22">(H105-0.6078)/1.3756</f>
+        <f t="shared" ref="U105" si="25">(H105-0.6078)/1.3756</f>
         <v>6.8277115440535052</v>
       </c>
       <c r="V105" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.3738005234079678</v>
       </c>
       <c r="W105" s="32">
@@ -4525,7 +4576,7 @@
         <v>5.3738005234079678</v>
       </c>
       <c r="X105" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>7.5546670543762735</v>
       </c>
     </row>
@@ -4572,7 +4623,7 @@
         <v>10</v>
       </c>
       <c r="E107" s="33">
-        <f t="shared" ref="E107:E108" si="23">(H107-0.6078)/1.3756</f>
+        <f t="shared" ref="E107:E108" si="26">(H107-0.6078)/1.3756</f>
         <v>22.093777260831637</v>
       </c>
       <c r="H107" s="3">
@@ -4604,7 +4655,7 @@
         <v>10</v>
       </c>
       <c r="E108" s="33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>4.6468450130851995</v>
       </c>
       <c r="H108" s="3">

</xml_diff>